<commit_message>
fix loi uc cap nhat thulai.xlsx
</commit_message>
<xml_diff>
--- a/insoden/thulai.xlsx
+++ b/insoden/thulai.xlsx
@@ -178,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -201,38 +201,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -306,6 +280,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -324,13 +301,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -675,7 +646,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,15 +1165,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1210,10 +1181,10 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
         <v>3</v>
@@ -1232,15 +1203,15 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
@@ -1252,33 +1223,33 @@
       <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="25"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:9" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="31"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1299,8 +1270,8 @@
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:9" s="18" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -1329,16 +1300,10 @@
       <c r="A13" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="24" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="24"/>
-      <c r="E13" s="24" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="E13" s="24"/>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
     </row>

</xml_diff>

<commit_message>
cap nhat thu lai
</commit_message>
<xml_diff>
--- a/insoden/thulai.xlsx
+++ b/insoden/thulai.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -96,6 +96,9 @@
   <si>
     <t>GIẤY ĐỀ NGHỊ THU LÃI</t>
   </si>
+  <si>
+    <t>Loại Tiền</t>
+  </si>
 </sst>
 </file>
 
@@ -105,7 +108,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +172,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -218,7 +234,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -237,9 +252,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -277,32 +289,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -646,7 +674,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,15 +1193,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1181,20 +1209,21 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
     </row>
     <row r="4" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
@@ -1203,171 +1232,181 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-    </row>
-    <row r="7" spans="1:9" s="10" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:9" s="9" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+    </row>
+    <row r="8" spans="1:9" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-    </row>
-    <row r="12" spans="1:9" s="18" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="30"/>
+    </row>
+    <row r="12" spans="1:9" s="16" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
+      <c r="H12" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="24" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="25" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="23"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="5"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="27"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="23"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="27"/>
+      <c r="F19" s="25"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -1376,7 +1415,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="27"/>
+      <c r="F20" s="25"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -1385,20 +1424,22 @@
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="27"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="E3:H3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.52" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>